<commit_message>
add: code capt & add skripsi 4
</commit_message>
<xml_diff>
--- a/DOKUMENT/rangkupam.xlsx
+++ b/DOKUMENT/rangkupam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\CODING LAIN\thesis\DOKUMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKRIPSI\DOKUMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99658074-9618-4D47-B509-0B46391B284C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E050521-E64D-4D2A-84B4-64132261BB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{082D9397-1B1B-4B71-8954-A9D7E17799A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{082D9397-1B1B-4B71-8954-A9D7E17799A7}"/>
   </bookViews>
   <sheets>
     <sheet name="model awal" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,12 +281,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,8 +561,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -582,24 +574,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,75 +619,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D7A5C3-4302-4427-86D5-33E45D3D5E2A}">
   <dimension ref="E2:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="152" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="152" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1031,18 +1034,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="5"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="5"/>
-      <c r="K2" s="21" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="K2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E3" s="5"/>
@@ -1085,27 +1088,27 @@
       </c>
     </row>
     <row r="5" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="55">
         <v>175</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="55">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="55">
         <v>125</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="55">
         <v>0.83</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="14">
+      <c r="J5" s="51"/>
+      <c r="K5" s="55">
         <v>0.83899999999999997</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14" t="s">
+      <c r="L5" s="55"/>
+      <c r="M5" s="55" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1158,13 +1161,13 @@
       </c>
     </row>
     <row r="9" spans="5:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
     </row>
     <row r="10" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F10" s="1" t="s">
@@ -1173,8 +1176,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F2:H2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="E2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1185,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16F24B3-4B99-49F3-AA16-7769F65F4673}">
   <dimension ref="B3:Q18"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="E1" zoomScale="116" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1214,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="26" t="s">
         <v>22</v>
       </c>
@@ -1232,7 +1235,7 @@
       <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1295,7 @@
       <c r="F5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="27">
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1327,27 +1330,27 @@
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="27" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="3">
         <v>240</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="23" t="s">
+      <c r="G6" s="28"/>
+      <c r="H6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="27" t="s">
         <v>38</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="23">
+      <c r="K6" s="27">
         <v>416</v>
       </c>
       <c r="M6" s="3">
@@ -1370,17 +1373,17 @@
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="23">
+      <c r="C7" s="29"/>
+      <c r="D7" s="27">
         <v>256</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="26"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="28"/>
       <c r="M7" s="3">
         <v>172</v>
       </c>
@@ -1404,14 +1407,14 @@
       <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="26"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="28"/>
       <c r="M8" s="3">
         <v>116</v>
       </c>
@@ -1435,14 +1438,14 @@
       <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="26"/>
-      <c r="K9" s="24"/>
+      <c r="K9" s="28"/>
       <c r="M9" s="7">
         <v>143</v>
       </c>
@@ -1466,14 +1469,14 @@
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="26"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="28"/>
       <c r="M10" s="3">
         <v>195</v>
       </c>
@@ -1494,19 +1497,19 @@
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="23" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27" t="s">
         <v>48</v>
       </c>
       <c r="J11" s="26"/>
-      <c r="K11" s="24"/>
+      <c r="K11" s="28"/>
       <c r="M11" s="3">
         <v>67</v>
       </c>
@@ -1527,17 +1530,17 @@
       <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="3">
         <v>48</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="26"/>
-      <c r="K12" s="24"/>
+      <c r="K12" s="28"/>
       <c r="M12" s="3">
         <v>115</v>
       </c>
@@ -1558,19 +1561,19 @@
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="23">
+      <c r="F13" s="28"/>
+      <c r="G13" s="27">
         <v>16</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="26"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="28"/>
       <c r="M13" s="3">
         <v>159</v>
       </c>
@@ -1591,19 +1594,19 @@
       <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="3" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="K14" s="25"/>
+      <c r="K14" s="29"/>
       <c r="M14" s="3">
         <v>172</v>
       </c>
@@ -1621,29 +1624,21 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="18" spans="8:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="K6:K14"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="J5:J14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="I11:I13"/>
@@ -1653,6 +1648,14 @@
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H6:H14"/>
     <mergeCell ref="G5:G11"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="K6:K14"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="J5:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1679,22 +1682,22 @@
   <sheetData>
     <row r="4" spans="4:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D4" s="26"/>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="27" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="29"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="33"/>
       <c r="S4" s="10"/>
     </row>
     <row r="5" spans="4:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -1740,7 +1743,7 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="4">
@@ -1781,7 +1784,7 @@
       <c r="D7" s="4">
         <v>2</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="4">
@@ -1814,7 +1817,7 @@
       <c r="D8" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="4">
@@ -1847,7 +1850,7 @@
       <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="4">
@@ -1880,7 +1883,7 @@
       <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="4">
@@ -1913,7 +1916,7 @@
       <c r="D11" s="4">
         <v>6</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="16" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="4">
@@ -1946,7 +1949,7 @@
       <c r="D12" s="4">
         <v>7</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="4">
@@ -1979,7 +1982,7 @@
       <c r="D13" s="4">
         <v>8</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F13" s="4">
@@ -2012,7 +2015,7 @@
       <c r="D14" s="4">
         <v>9</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="4">
@@ -2045,7 +2048,7 @@
       <c r="D15" s="4">
         <v>10</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="4">
@@ -2076,22 +2079,22 @@
     </row>
     <row r="17" spans="1:74" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17" s="26"/>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="27" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="33"/>
     </row>
     <row r="18" spans="1:74" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D18" s="26"/>
@@ -2136,28 +2139,28 @@
       <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>61</v>
       </c>
       <c r="F19" s="4">
         <v>240</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="27">
         <v>1E-4</v>
       </c>
       <c r="I19" s="4">
         <v>16</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="27">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K19" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="27">
         <v>200</v>
       </c>
       <c r="M19" s="3"/>
@@ -2173,22 +2176,22 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="4">
         <v>240</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="4">
         <v>16</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="28"/>
       <c r="K20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L20" s="24"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3">
@@ -2202,22 +2205,22 @@
       <c r="D21" s="4">
         <v>3</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="4">
         <v>240</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="4">
         <v>32</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="28"/>
       <c r="K21" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L21" s="24"/>
+      <c r="L21" s="28"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3">
@@ -2231,22 +2234,22 @@
       <c r="D22" s="4">
         <v>4</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F22" s="4">
         <v>240</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="4">
         <v>32</v>
       </c>
-      <c r="J22" s="24"/>
+      <c r="J22" s="28"/>
       <c r="K22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="24"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3">
@@ -2263,22 +2266,22 @@
       <c r="D23" s="12">
         <v>5</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="12">
         <v>240</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="12">
         <v>64</v>
       </c>
-      <c r="J23" s="24"/>
+      <c r="J23" s="28"/>
       <c r="K23" s="12">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L23" s="24"/>
+      <c r="L23" s="28"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7">
@@ -2350,22 +2353,22 @@
       <c r="D24" s="4">
         <v>6</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>61</v>
       </c>
       <c r="F24" s="4">
         <v>256</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="4">
         <v>64</v>
       </c>
-      <c r="J24" s="24"/>
+      <c r="J24" s="28"/>
       <c r="K24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L24" s="24"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3">
@@ -2379,22 +2382,22 @@
       <c r="D25" s="4">
         <v>7</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F25" s="4">
         <v>256</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="4">
         <v>16</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="28"/>
       <c r="K25" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L25" s="24"/>
+      <c r="L25" s="28"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3">
@@ -2408,22 +2411,22 @@
       <c r="D26" s="4">
         <v>8</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="4">
         <v>256</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="4">
         <v>16</v>
       </c>
-      <c r="J26" s="24"/>
+      <c r="J26" s="28"/>
       <c r="K26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L26" s="24"/>
+      <c r="L26" s="28"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3">
@@ -2437,22 +2440,22 @@
       <c r="D27" s="4">
         <v>9</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F27" s="4">
         <v>256</v>
       </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="4">
         <v>32</v>
       </c>
-      <c r="J27" s="24"/>
+      <c r="J27" s="28"/>
       <c r="K27" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L27" s="24"/>
+      <c r="L27" s="28"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3">
@@ -2466,22 +2469,22 @@
       <c r="D28" s="4">
         <v>10</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F28" s="4">
         <v>256</v>
       </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="4">
         <v>32</v>
       </c>
-      <c r="J28" s="25"/>
+      <c r="J28" s="29"/>
       <c r="K28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L28" s="25"/>
+      <c r="L28" s="29"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3">
@@ -2492,7 +2495,7 @@
       </c>
     </row>
     <row r="32" spans="1:74" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="18" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2527,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B3C22-B1D8-4A1D-8A98-F695002041FD}">
   <dimension ref="E4:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="X7" sqref="X7:Z7"/>
     </sheetView>
   </sheetViews>
@@ -2535,1032 +2538,1009 @@
   <sheetData>
     <row r="4" spans="5:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="5:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="36" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="38"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="36"/>
     </row>
     <row r="6" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="36" t="s">
+      <c r="G6" s="36"/>
+      <c r="H6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="36" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="31" t="s">
+      <c r="K6" s="36"/>
+      <c r="L6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="36" t="s">
+      <c r="N6" s="36"/>
+      <c r="O6" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="36" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="38"/>
-      <c r="S6" s="31" t="s">
+      <c r="R6" s="36"/>
+      <c r="S6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="36" t="s">
+      <c r="T6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="38"/>
-      <c r="V6" s="36" t="s">
+      <c r="U6" s="36"/>
+      <c r="V6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="38"/>
-      <c r="X6" s="36" t="s">
+      <c r="W6" s="36"/>
+      <c r="X6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="32"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="21"/>
     </row>
     <row r="7" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="34">
         <v>240</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39" t="s">
+      <c r="G7" s="36"/>
+      <c r="H7" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="39">
+      <c r="I7" s="43"/>
+      <c r="J7" s="42">
         <v>1E-4</v>
       </c>
-      <c r="K7" s="40"/>
-      <c r="L7" s="31">
+      <c r="K7" s="43"/>
+      <c r="L7" s="20">
         <v>16</v>
       </c>
-      <c r="M7" s="39">
+      <c r="M7" s="42">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="N7" s="40"/>
-      <c r="O7" s="36">
+      <c r="N7" s="43"/>
+      <c r="O7" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="39">
+      <c r="P7" s="36"/>
+      <c r="Q7" s="42">
         <v>200</v>
       </c>
-      <c r="R7" s="40"/>
-      <c r="S7" s="31">
+      <c r="R7" s="43"/>
+      <c r="S7" s="20">
         <v>83</v>
       </c>
-      <c r="T7" s="36">
+      <c r="T7" s="34">
         <v>0.86</v>
       </c>
-      <c r="U7" s="38"/>
-      <c r="V7" s="36">
+      <c r="U7" s="36"/>
+      <c r="V7" s="34">
         <v>16</v>
       </c>
-      <c r="W7" s="38"/>
-      <c r="X7" s="36">
+      <c r="W7" s="36"/>
+      <c r="X7" s="34">
         <v>0.88061</v>
       </c>
-      <c r="Y7" s="37"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="32"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="36"/>
+      <c r="AA7" s="21"/>
     </row>
     <row r="8" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="34">
         <v>240</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="31">
+      <c r="G8" s="36"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="20">
         <v>16</v>
       </c>
-      <c r="M8" s="41"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="36" t="s">
+      <c r="M8" s="44"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="31">
+      <c r="P8" s="36"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="20">
         <v>199</v>
       </c>
-      <c r="T8" s="36">
+      <c r="T8" s="34">
         <v>0.875</v>
       </c>
-      <c r="U8" s="38"/>
-      <c r="V8" s="36">
+      <c r="U8" s="36"/>
+      <c r="V8" s="34">
         <v>150</v>
       </c>
-      <c r="W8" s="38"/>
-      <c r="X8" s="36">
+      <c r="W8" s="36"/>
+      <c r="X8" s="34">
         <v>0.87702999999999998</v>
       </c>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="32"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="21"/>
     </row>
     <row r="9" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="34">
         <v>240</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="31">
+      <c r="G9" s="36"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="20">
         <v>32</v>
       </c>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="36">
+      <c r="M9" s="44"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="31">
+      <c r="P9" s="36"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="20">
         <v>103</v>
       </c>
-      <c r="T9" s="36">
+      <c r="T9" s="34">
         <v>0.875</v>
       </c>
-      <c r="U9" s="38"/>
-      <c r="V9" s="36">
+      <c r="U9" s="36"/>
+      <c r="V9" s="34">
         <v>85</v>
       </c>
-      <c r="W9" s="38"/>
-      <c r="X9" s="36">
+      <c r="W9" s="36"/>
+      <c r="X9" s="34">
         <v>0.88134999999999997</v>
       </c>
-      <c r="Y9" s="37"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="32"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="36"/>
+      <c r="AA9" s="21"/>
     </row>
     <row r="10" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="34">
         <v>240</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="31">
+      <c r="G10" s="36"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="20">
         <v>32</v>
       </c>
-      <c r="M10" s="41"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="36" t="s">
+      <c r="M10" s="44"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="31">
+      <c r="P10" s="36"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="20">
         <v>150</v>
       </c>
-      <c r="T10" s="36">
+      <c r="T10" s="34">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U10" s="38"/>
-      <c r="V10" s="36">
+      <c r="U10" s="36"/>
+      <c r="V10" s="34">
         <v>78</v>
       </c>
-      <c r="W10" s="38"/>
-      <c r="X10" s="36">
+      <c r="W10" s="36"/>
+      <c r="X10" s="34">
         <v>0.88275000000000003</v>
       </c>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="32"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="21"/>
     </row>
     <row r="11" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="34">
         <v>240</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="31">
+      <c r="G11" s="36"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="20">
         <v>64</v>
       </c>
-      <c r="M11" s="41"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="36">
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="31">
+      <c r="P11" s="36"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="20">
         <v>199</v>
       </c>
-      <c r="T11" s="36">
+      <c r="T11" s="34">
         <v>0.874</v>
       </c>
-      <c r="U11" s="38"/>
-      <c r="V11" s="36">
+      <c r="U11" s="36"/>
+      <c r="V11" s="34">
         <v>147</v>
       </c>
-      <c r="W11" s="38"/>
-      <c r="X11" s="36">
+      <c r="W11" s="36"/>
+      <c r="X11" s="34">
         <v>0.87795000000000001</v>
       </c>
-      <c r="Y11" s="37"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="32"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="21"/>
     </row>
     <row r="12" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="34">
         <v>240</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="31">
+      <c r="G12" s="36"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="20">
         <v>64</v>
       </c>
-      <c r="M12" s="41"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="36" t="s">
+      <c r="M12" s="44"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="31">
+      <c r="P12" s="36"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="20">
         <v>114</v>
       </c>
-      <c r="T12" s="36">
+      <c r="T12" s="34">
         <v>0.85899999999999999</v>
       </c>
-      <c r="U12" s="38"/>
-      <c r="V12" s="36">
+      <c r="U12" s="36"/>
+      <c r="V12" s="34">
         <v>59</v>
       </c>
-      <c r="W12" s="38"/>
-      <c r="X12" s="36">
+      <c r="W12" s="36"/>
+      <c r="X12" s="34">
         <v>0.87651000000000001</v>
       </c>
-      <c r="Y12" s="37"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="32"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="21"/>
     </row>
     <row r="13" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="34">
         <v>256</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="31">
+      <c r="G13" s="36"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="20">
         <v>16</v>
       </c>
-      <c r="M13" s="41"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="36">
+      <c r="M13" s="44"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="31">
+      <c r="P13" s="36"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="20">
         <v>83</v>
       </c>
-      <c r="T13" s="36">
+      <c r="T13" s="34">
         <v>0.86</v>
       </c>
-      <c r="U13" s="38"/>
-      <c r="V13" s="36">
+      <c r="U13" s="36"/>
+      <c r="V13" s="34">
         <v>16</v>
       </c>
-      <c r="W13" s="38"/>
-      <c r="X13" s="36">
+      <c r="W13" s="36"/>
+      <c r="X13" s="34">
         <v>0.88161</v>
       </c>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="38"/>
-      <c r="AA13" s="32"/>
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="21"/>
     </row>
     <row r="14" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="34">
         <v>256</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="31">
+      <c r="G14" s="36"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="20">
         <v>16</v>
       </c>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="36" t="s">
+      <c r="M14" s="44"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="31">
+      <c r="P14" s="36"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="20">
         <v>199</v>
       </c>
-      <c r="T14" s="36">
+      <c r="T14" s="34">
         <v>0.875</v>
       </c>
-      <c r="U14" s="38"/>
-      <c r="V14" s="36">
+      <c r="U14" s="36"/>
+      <c r="V14" s="34">
         <v>150</v>
       </c>
-      <c r="W14" s="38"/>
-      <c r="X14" s="36">
+      <c r="W14" s="36"/>
+      <c r="X14" s="34">
         <v>0.87702999999999998</v>
       </c>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="32"/>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="21"/>
     </row>
     <row r="15" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="34">
         <v>256</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="31">
+      <c r="G15" s="36"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="20">
         <v>32</v>
       </c>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="36">
+      <c r="M15" s="44"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="31">
+      <c r="P15" s="36"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="20">
         <v>103</v>
       </c>
-      <c r="T15" s="36">
+      <c r="T15" s="34">
         <v>0.875</v>
       </c>
-      <c r="U15" s="38"/>
-      <c r="V15" s="36">
+      <c r="U15" s="36"/>
+      <c r="V15" s="34">
         <v>85</v>
       </c>
-      <c r="W15" s="38"/>
-      <c r="X15" s="36">
+      <c r="W15" s="36"/>
+      <c r="X15" s="34">
         <v>0.88134999999999997</v>
       </c>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="32"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="21"/>
     </row>
     <row r="16" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="34">
         <v>256</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="31">
+      <c r="G16" s="36"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="20">
         <v>32</v>
       </c>
-      <c r="M16" s="43"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="36" t="s">
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="31">
+      <c r="P16" s="36"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="20">
         <v>130</v>
       </c>
-      <c r="T16" s="36">
+      <c r="T16" s="34">
         <v>0.86799999999999999</v>
       </c>
-      <c r="U16" s="38"/>
-      <c r="V16" s="36">
+      <c r="U16" s="36"/>
+      <c r="V16" s="34">
         <v>78</v>
       </c>
-      <c r="W16" s="38"/>
-      <c r="X16" s="36">
+      <c r="W16" s="36"/>
+      <c r="X16" s="34">
         <v>0.88275000000000003</v>
       </c>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="32"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="21"/>
     </row>
     <row r="17" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="36" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="45"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="38"/>
     </row>
     <row r="18" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="36" t="s">
+      <c r="H18" s="36"/>
+      <c r="I18" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="36" t="s">
+      <c r="J18" s="36"/>
+      <c r="K18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="37"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="36" t="s">
+      <c r="L18" s="35"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="38"/>
-      <c r="P18" s="36" t="s">
+      <c r="O18" s="36"/>
+      <c r="P18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="31" t="s">
+      <c r="Q18" s="36"/>
+      <c r="R18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="S18" s="36" t="s">
+      <c r="S18" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="T18" s="38"/>
-      <c r="U18" s="36" t="s">
+      <c r="T18" s="36"/>
+      <c r="U18" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="V18" s="38"/>
-      <c r="W18" s="36" t="s">
+      <c r="V18" s="36"/>
+      <c r="W18" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="31" t="s">
+      <c r="X18" s="36"/>
+      <c r="Y18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="Z18" s="46"/>
-      <c r="AA18" s="45"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="38"/>
     </row>
     <row r="19" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="20">
         <v>240</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="39">
+      <c r="H19" s="43"/>
+      <c r="I19" s="42">
         <v>1E-4</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="36">
+      <c r="J19" s="43"/>
+      <c r="K19" s="34">
         <v>16</v>
       </c>
-      <c r="L19" s="37"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="39">
+      <c r="L19" s="35"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="42">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="36">
+      <c r="O19" s="43"/>
+      <c r="P19" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="47">
+      <c r="Q19" s="36"/>
+      <c r="R19" s="48">
         <v>200</v>
       </c>
-      <c r="S19" s="36"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="36">
+      <c r="S19" s="34"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="34">
         <v>24</v>
       </c>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="31">
+      <c r="X19" s="36"/>
+      <c r="Y19" s="20">
         <v>0.87990000000000002</v>
       </c>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="45"/>
+      <c r="Z19" s="37"/>
+      <c r="AA19" s="38"/>
     </row>
     <row r="20" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="20">
         <v>240</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="36">
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="34">
         <v>16</v>
       </c>
-      <c r="L20" s="37"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="36" t="s">
+      <c r="L20" s="35"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="36">
+      <c r="Q20" s="36"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="34">
         <v>38</v>
       </c>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="31">
+      <c r="X20" s="36"/>
+      <c r="Y20" s="20">
         <v>0.88602999999999998</v>
       </c>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="45"/>
+      <c r="Z20" s="37"/>
+      <c r="AA20" s="38"/>
     </row>
     <row r="21" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="20">
         <v>240</v>
       </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="36">
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="34">
         <v>32</v>
       </c>
-      <c r="L21" s="37"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="36">
+      <c r="L21" s="35"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="36">
+      <c r="Q21" s="36"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="34">
         <v>168</v>
       </c>
-      <c r="X21" s="38"/>
-      <c r="Y21" s="31">
+      <c r="X21" s="36"/>
+      <c r="Y21" s="20">
         <v>0.88941999999999999</v>
       </c>
-      <c r="Z21" s="46"/>
-      <c r="AA21" s="45"/>
+      <c r="Z21" s="37"/>
+      <c r="AA21" s="38"/>
     </row>
     <row r="22" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="20">
         <v>240</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="36">
+      <c r="G22" s="44"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="34">
         <v>32</v>
       </c>
-      <c r="L22" s="37"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="36" t="s">
+      <c r="L22" s="35"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="36">
+      <c r="Q22" s="36"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="34">
         <v>29</v>
       </c>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="31">
+      <c r="X22" s="36"/>
+      <c r="Y22" s="20">
         <v>0.88482000000000005</v>
       </c>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="45"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="38"/>
     </row>
     <row r="23" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="24">
         <v>240</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="50">
+      <c r="G23" s="44"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="39">
         <v>64</v>
       </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="50">
+      <c r="L23" s="40"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="39">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="50"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="50">
+      <c r="Q23" s="41"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="39">
         <v>65</v>
       </c>
-      <c r="X23" s="52"/>
-      <c r="Y23" s="35">
+      <c r="X23" s="41"/>
+      <c r="Y23" s="24">
         <v>0.88971</v>
       </c>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="45"/>
+      <c r="Z23" s="37"/>
+      <c r="AA23" s="38"/>
     </row>
     <row r="24" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="20">
         <v>256</v>
       </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="36">
+      <c r="G24" s="44"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="34">
         <v>64</v>
       </c>
-      <c r="L24" s="37"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="36" t="s">
+      <c r="L24" s="35"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="36">
+      <c r="Q24" s="36"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="34">
         <v>178</v>
       </c>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="31">
+      <c r="X24" s="36"/>
+      <c r="Y24" s="20">
         <v>0.88748000000000005</v>
       </c>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="45"/>
+      <c r="Z24" s="37"/>
+      <c r="AA24" s="38"/>
     </row>
     <row r="25" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="20">
         <v>256</v>
       </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="36">
+      <c r="G25" s="44"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="34">
         <v>16</v>
       </c>
-      <c r="L25" s="37"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="36">
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="48"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="36"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="36">
+      <c r="Q25" s="36"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="34">
         <v>24</v>
       </c>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="31">
+      <c r="X25" s="36"/>
+      <c r="Y25" s="20">
         <v>0.87990000000000002</v>
       </c>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="45"/>
+      <c r="Z25" s="37"/>
+      <c r="AA25" s="38"/>
     </row>
     <row r="26" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="20">
         <v>256</v>
       </c>
-      <c r="G26" s="41"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="36">
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="34">
         <v>16</v>
       </c>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="36" t="s">
+      <c r="L26" s="35"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="48"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="36"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="36">
+      <c r="Q26" s="36"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="34">
         <v>38</v>
       </c>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="31">
+      <c r="X26" s="36"/>
+      <c r="Y26" s="20">
         <v>0.88602999999999998</v>
       </c>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="45"/>
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="38"/>
     </row>
     <row r="27" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="20">
         <v>256</v>
       </c>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="36">
+      <c r="G27" s="44"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="34">
         <v>32</v>
       </c>
-      <c r="L27" s="37"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="36">
+      <c r="L27" s="35"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="34">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="38"/>
-      <c r="W27" s="36">
+      <c r="Q27" s="36"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="34">
         <v>29</v>
       </c>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="31">
+      <c r="X27" s="36"/>
+      <c r="Y27" s="20">
         <v>0.87646000000000002</v>
       </c>
-      <c r="Z27" s="46"/>
-      <c r="AA27" s="45"/>
+      <c r="Z27" s="37"/>
+      <c r="AA27" s="38"/>
     </row>
     <row r="28" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="20">
         <v>256</v>
       </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="36">
+      <c r="G28" s="46"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="34">
         <v>32</v>
       </c>
-      <c r="L28" s="37"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="36" t="s">
+      <c r="L28" s="35"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="38"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="38"/>
-      <c r="W28" s="36">
+      <c r="Q28" s="36"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="34">
         <v>70</v>
       </c>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="31">
+      <c r="X28" s="36"/>
+      <c r="Y28" s="20">
         <v>0.87980000000000003</v>
       </c>
-      <c r="Z28" s="46"/>
-      <c r="AA28" s="45"/>
+      <c r="Z28" s="37"/>
+      <c r="AA28" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="G19:H28"/>
-    <mergeCell ref="I19:J28"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:O28"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:R28"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="E5:R5"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I16"/>
+    <mergeCell ref="J7:K16"/>
+    <mergeCell ref="M7:N16"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R16"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Z8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:Z13"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="T16:U16"/>
@@ -3579,56 +3559,79 @@
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Z8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I16"/>
-    <mergeCell ref="J7:K16"/>
-    <mergeCell ref="M7:N16"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R16"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="E5:R5"/>
-    <mergeCell ref="S5:AA5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="G19:H28"/>
+    <mergeCell ref="I19:J28"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:O28"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:R28"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="Z27:AA27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: bab 4 & 5
</commit_message>
<xml_diff>
--- a/DOKUMENT/rangkupam.xlsx
+++ b/DOKUMENT/rangkupam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKRIPSI\DOKUMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7712881-0E33-4A4F-8D5F-1C9257AE4212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27CC075-7DF7-4022-BF60-0F42EC877319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{082D9397-1B1B-4B71-8954-A9D7E17799A7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="80">
   <si>
     <t>Model 1</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>precis</t>
+  </si>
+  <si>
+    <t>rata-rata</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -642,6 +645,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,8 +666,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -666,8 +678,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -685,21 +700,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -720,6 +720,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,26 +735,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2226,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D7A5C3-4302-4427-86D5-33E45D3D5E2A}">
   <dimension ref="E2:V17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2243,18 +2237,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="K2" s="26" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="K2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E3" s="5"/>
@@ -2475,6 +2469,15 @@
       </c>
       <c r="V7" s="1">
         <v>0.79</v>
+      </c>
+    </row>
+    <row r="8" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="1">
+        <f>AVERAGE(I4:I7)</f>
+        <v>0.83099999999999996</v>
       </c>
     </row>
     <row r="9" spans="5:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,28 +2649,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="M3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="M3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2727,7 +2730,7 @@
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="34">
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -2736,7 +2739,7 @@
       <c r="I5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="37">
         <v>200</v>
       </c>
       <c r="K5" s="3">
@@ -2762,27 +2765,27 @@
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="34" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="3">
         <v>240</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31" t="s">
+      <c r="G6" s="35"/>
+      <c r="H6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31">
+      <c r="J6" s="37"/>
+      <c r="K6" s="34">
         <v>416</v>
       </c>
       <c r="M6" s="3">
@@ -2805,17 +2808,17 @@
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="31">
+      <c r="C7" s="36"/>
+      <c r="D7" s="34">
         <v>256</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="32"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="35"/>
       <c r="M7" s="3">
         <v>172</v>
       </c>
@@ -2839,14 +2842,14 @@
       <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="32"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="35"/>
       <c r="M8" s="3">
         <v>116</v>
       </c>
@@ -2870,14 +2873,14 @@
       <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="32"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="35"/>
       <c r="M9" s="7">
         <v>143</v>
       </c>
@@ -2901,14 +2904,14 @@
       <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="32"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="35"/>
       <c r="M10" s="3">
         <v>195</v>
       </c>
@@ -2929,19 +2932,19 @@
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="31" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="32"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="35"/>
       <c r="M11" s="3">
         <v>67</v>
       </c>
@@ -2962,17 +2965,17 @@
       <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="32"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="3">
         <v>48</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="32"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="35"/>
       <c r="M12" s="3">
         <v>115</v>
       </c>
@@ -2993,19 +2996,19 @@
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="31">
+      <c r="F13" s="35"/>
+      <c r="G13" s="34">
         <v>16</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="32"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="35"/>
       <c r="M13" s="3">
         <v>159</v>
       </c>
@@ -3026,19 +3029,19 @@
       <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="33"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="36"/>
       <c r="M14" s="3">
         <v>172</v>
       </c>
@@ -3056,21 +3059,29 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="18" spans="8:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="K6:K14"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="J5:J14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="I11:I13"/>
@@ -3080,14 +3091,6 @@
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H6:H14"/>
     <mergeCell ref="G5:G11"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="K6:K14"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="J5:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3097,8 +3100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB8005-5696-4015-A771-D6400CC063DD}">
   <dimension ref="A4:BV34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,27 +3128,27 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="30"/>
-      <c r="E4" s="35" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="35" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="37"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="41"/>
       <c r="S4" s="10"/>
     </row>
     <row r="5" spans="4:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="30"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -3193,22 +3196,22 @@
       <c r="F6" s="4">
         <v>240</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="37">
         <v>1E-4</v>
       </c>
       <c r="I6" s="4">
         <v>16</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="37">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K6" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="37">
         <v>200</v>
       </c>
       <c r="M6" s="3">
@@ -3234,16 +3237,16 @@
       <c r="F7" s="4">
         <v>240</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="4">
         <v>16</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="30"/>
+      <c r="L7" s="37"/>
       <c r="M7" s="3">
         <v>199</v>
       </c>
@@ -3267,16 +3270,16 @@
       <c r="F8" s="4">
         <v>240</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="4">
         <v>32</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L8" s="30"/>
+      <c r="L8" s="37"/>
       <c r="M8" s="3">
         <v>103</v>
       </c>
@@ -3300,16 +3303,16 @@
       <c r="F9" s="4">
         <v>240</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="4">
         <v>32</v>
       </c>
-      <c r="J9" s="30"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="30"/>
+      <c r="L9" s="37"/>
       <c r="M9" s="3">
         <v>150</v>
       </c>
@@ -3333,16 +3336,16 @@
       <c r="F10" s="4">
         <v>240</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="4">
         <v>64</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="37"/>
       <c r="K10" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L10" s="30"/>
+      <c r="L10" s="37"/>
       <c r="M10" s="3">
         <v>199</v>
       </c>
@@ -3366,16 +3369,16 @@
       <c r="F11" s="4">
         <v>240</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="4">
         <v>64</v>
       </c>
-      <c r="J11" s="30"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="30"/>
+      <c r="L11" s="37"/>
       <c r="M11" s="3">
         <v>114</v>
       </c>
@@ -3399,16 +3402,16 @@
       <c r="F12" s="4">
         <v>256</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="4">
         <v>16</v>
       </c>
-      <c r="J12" s="30"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L12" s="30"/>
+      <c r="L12" s="37"/>
       <c r="M12" s="3">
         <v>83</v>
       </c>
@@ -3432,16 +3435,16 @@
       <c r="F13" s="4">
         <v>256</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="4">
         <v>16</v>
       </c>
-      <c r="J13" s="30"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="30"/>
+      <c r="L13" s="37"/>
       <c r="M13" s="3">
         <v>199</v>
       </c>
@@ -3465,16 +3468,16 @@
       <c r="F14" s="4">
         <v>256</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="4">
         <v>32</v>
       </c>
-      <c r="J14" s="30"/>
+      <c r="J14" s="37"/>
       <c r="K14" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L14" s="30"/>
+      <c r="L14" s="37"/>
       <c r="M14" s="3">
         <v>103</v>
       </c>
@@ -3498,16 +3501,16 @@
       <c r="F15" s="4">
         <v>256</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="4">
         <v>32</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="37"/>
       <c r="K15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L15" s="30"/>
+      <c r="L15" s="37"/>
       <c r="M15" s="3">
         <v>130</v>
       </c>
@@ -3522,42 +3525,42 @@
       </c>
     </row>
     <row r="17" spans="1:74" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="30"/>
-      <c r="E17" s="35" t="s">
+      <c r="D17" s="37"/>
+      <c r="E17" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="35" t="s">
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="37"/>
-      <c r="S17" s="60" t="s">
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="41"/>
+      <c r="S17" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="T17" s="60"/>
-      <c r="U17" s="60"/>
-      <c r="V17" s="60"/>
-      <c r="W17" s="60"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="60"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="60" t="s">
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="AB17" s="60"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="60"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
     </row>
     <row r="18" spans="1:74" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="30"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="4" t="s">
         <v>14</v>
       </c>
@@ -3594,43 +3597,43 @@
       <c r="P18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S18" s="58" t="s">
+      <c r="S18" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="T18" s="58" t="s">
+      <c r="T18" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="U18" s="58" t="s">
+      <c r="U18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="V18" s="58" t="s">
+      <c r="V18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="W18" s="58" t="s">
+      <c r="W18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="X18" s="58" t="s">
+      <c r="X18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="Y18" s="58" t="s">
+      <c r="Y18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="Z18" s="58" t="s">
+      <c r="Z18" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AA18" s="59" t="s">
+      <c r="AA18" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AB18" s="59" t="s">
+      <c r="AB18" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AC18" s="59" t="s">
+      <c r="AC18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AD18" s="59" t="s">
+      <c r="AD18" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="AE18" s="61" t="s">
+      <c r="AE18" s="28" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3644,22 +3647,22 @@
       <c r="F19" s="4">
         <v>240</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="34">
         <v>1E-4</v>
       </c>
       <c r="I19" s="4">
         <v>16</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="34">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K19" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L19" s="31">
+      <c r="L19" s="34">
         <v>200</v>
       </c>
       <c r="M19" s="3">
@@ -3674,40 +3677,40 @@
       <c r="P19" s="3">
         <v>0.87990000000000002</v>
       </c>
-      <c r="S19" s="57" t="s">
+      <c r="S19" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="T19" s="55">
+      <c r="T19" s="4">
         <v>240</v>
       </c>
       <c r="U19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V19" s="31">
+      <c r="V19" s="34">
         <v>1E-4</v>
       </c>
-      <c r="W19" s="55">
+      <c r="W19" s="4">
         <v>64</v>
       </c>
-      <c r="X19" s="31">
+      <c r="X19" s="34">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="Y19" s="55">
+      <c r="Y19" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z19" s="31">
+      <c r="Z19" s="34">
         <v>200</v>
       </c>
-      <c r="AA19" s="56">
+      <c r="AA19" s="3">
         <v>200</v>
       </c>
-      <c r="AB19" s="56">
+      <c r="AB19" s="3">
         <v>0.871</v>
       </c>
-      <c r="AC19" s="56">
+      <c r="AC19" s="3">
         <v>65</v>
       </c>
-      <c r="AD19" s="56">
+      <c r="AD19" s="3">
         <v>0.88971</v>
       </c>
     </row>
@@ -3721,16 +3724,16 @@
       <c r="F20" s="4">
         <v>240</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="4">
         <v>16</v>
       </c>
-      <c r="J20" s="32"/>
+      <c r="J20" s="35"/>
       <c r="K20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L20" s="32"/>
+      <c r="L20" s="35"/>
       <c r="M20" s="3">
         <v>199</v>
       </c>
@@ -3752,15 +3755,15 @@
       <c r="U20" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="V20" s="32"/>
+      <c r="V20" s="35"/>
       <c r="W20" s="4">
         <v>32</v>
       </c>
-      <c r="X20" s="32"/>
+      <c r="X20" s="35"/>
       <c r="Y20" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z20" s="32"/>
+      <c r="Z20" s="35"/>
       <c r="AA20" s="3">
         <v>200</v>
       </c>
@@ -3784,16 +3787,16 @@
       <c r="F21" s="4">
         <v>240</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="4">
         <v>32</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="35"/>
       <c r="K21" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L21" s="32"/>
+      <c r="L21" s="35"/>
       <c r="M21" s="3">
         <v>200</v>
       </c>
@@ -3815,15 +3818,15 @@
       <c r="U21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="V21" s="32"/>
+      <c r="V21" s="35"/>
       <c r="W21" s="4">
         <v>16</v>
       </c>
-      <c r="X21" s="32"/>
+      <c r="X21" s="35"/>
       <c r="Y21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z21" s="32"/>
+      <c r="Z21" s="35"/>
       <c r="AA21" s="3">
         <v>199</v>
       </c>
@@ -3847,16 +3850,16 @@
       <c r="F22" s="4">
         <v>240</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="4">
         <v>32</v>
       </c>
-      <c r="J22" s="32"/>
+      <c r="J22" s="35"/>
       <c r="K22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="32"/>
+      <c r="L22" s="35"/>
       <c r="M22" s="3">
         <v>66</v>
       </c>
@@ -3878,15 +3881,15 @@
       <c r="U22" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V22" s="32"/>
+      <c r="V22" s="35"/>
       <c r="W22" s="4">
         <v>32</v>
       </c>
-      <c r="X22" s="32"/>
+      <c r="X22" s="35"/>
       <c r="Y22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z22" s="32"/>
+      <c r="Z22" s="35"/>
       <c r="AA22" s="3">
         <v>66</v>
       </c>
@@ -3913,16 +3916,16 @@
       <c r="F23" s="12">
         <v>240</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
       <c r="I23" s="12">
         <v>64</v>
       </c>
-      <c r="J23" s="32"/>
+      <c r="J23" s="35"/>
       <c r="K23" s="12">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L23" s="32"/>
+      <c r="L23" s="35"/>
       <c r="M23" s="7">
         <v>200</v>
       </c>
@@ -3946,15 +3949,15 @@
       <c r="U23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V23" s="32"/>
+      <c r="V23" s="35"/>
       <c r="W23" s="4">
         <v>32</v>
       </c>
-      <c r="X23" s="32"/>
+      <c r="X23" s="35"/>
       <c r="Y23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z23" s="32"/>
+      <c r="Z23" s="35"/>
       <c r="AA23" s="3">
         <v>130</v>
       </c>
@@ -4022,16 +4025,16 @@
       <c r="F24" s="4">
         <v>256</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="4">
         <v>64</v>
       </c>
-      <c r="J24" s="32"/>
+      <c r="J24" s="35"/>
       <c r="K24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L24" s="32"/>
+      <c r="L24" s="35"/>
       <c r="M24" s="3">
         <v>200</v>
       </c>
@@ -4053,15 +4056,15 @@
       <c r="U24" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="V24" s="32"/>
+      <c r="V24" s="35"/>
       <c r="W24" s="4">
         <v>16</v>
       </c>
-      <c r="X24" s="32"/>
+      <c r="X24" s="35"/>
       <c r="Y24" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z24" s="32"/>
+      <c r="Z24" s="35"/>
       <c r="AA24" s="3">
         <v>83</v>
       </c>
@@ -4085,16 +4088,16 @@
       <c r="F25" s="4">
         <v>256</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="4">
         <v>16</v>
       </c>
-      <c r="J25" s="32"/>
+      <c r="J25" s="35"/>
       <c r="K25" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L25" s="32"/>
+      <c r="L25" s="35"/>
       <c r="M25" s="3">
         <v>116</v>
       </c>
@@ -4116,15 +4119,15 @@
       <c r="U25" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V25" s="32"/>
+      <c r="V25" s="35"/>
       <c r="W25" s="4">
         <v>32</v>
       </c>
-      <c r="X25" s="32"/>
+      <c r="X25" s="35"/>
       <c r="Y25" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z25" s="32"/>
+      <c r="Z25" s="35"/>
       <c r="AA25" s="3">
         <v>103</v>
       </c>
@@ -4148,16 +4151,16 @@
       <c r="F26" s="4">
         <v>256</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="4">
         <v>16</v>
       </c>
-      <c r="J26" s="32"/>
+      <c r="J26" s="35"/>
       <c r="K26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L26" s="32"/>
+      <c r="L26" s="35"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3">
@@ -4175,15 +4178,15 @@
       <c r="U26" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="V26" s="32"/>
+      <c r="V26" s="35"/>
       <c r="W26" s="4">
         <v>16</v>
       </c>
-      <c r="X26" s="32"/>
+      <c r="X26" s="35"/>
       <c r="Y26" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z26" s="32"/>
+      <c r="Z26" s="35"/>
       <c r="AA26" s="3">
         <v>116</v>
       </c>
@@ -4207,16 +4210,16 @@
       <c r="F27" s="4">
         <v>256</v>
       </c>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
       <c r="I27" s="4">
         <v>32</v>
       </c>
-      <c r="J27" s="32"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="L27" s="32"/>
+      <c r="L27" s="35"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3">
@@ -4234,15 +4237,15 @@
       <c r="U27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V27" s="32"/>
+      <c r="V27" s="35"/>
       <c r="W27" s="4">
         <v>16</v>
       </c>
-      <c r="X27" s="32"/>
+      <c r="X27" s="35"/>
       <c r="Y27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z27" s="32"/>
+      <c r="Z27" s="35"/>
       <c r="AA27" s="3">
         <v>199</v>
       </c>
@@ -4266,16 +4269,16 @@
       <c r="F28" s="4">
         <v>256</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="4">
         <v>32</v>
       </c>
-      <c r="J28" s="33"/>
+      <c r="J28" s="36"/>
       <c r="K28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L28" s="33"/>
+      <c r="L28" s="36"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3">
@@ -4293,15 +4296,15 @@
       <c r="U28" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="V28" s="33"/>
-      <c r="W28" s="55">
+      <c r="V28" s="36"/>
+      <c r="W28" s="4">
         <v>64</v>
       </c>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="55">
+      <c r="X28" s="36"/>
+      <c r="Y28" s="4">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z28" s="33"/>
+      <c r="Z28" s="36"/>
       <c r="AA28" s="3">
         <v>114</v>
       </c>
@@ -4330,11 +4333,6 @@
     <sortCondition descending="1" ref="AD19:AD28"/>
   </sortState>
   <mergeCells count="19">
-    <mergeCell ref="S17:Z17"/>
-    <mergeCell ref="AA17:AD17"/>
-    <mergeCell ref="V19:V28"/>
-    <mergeCell ref="X19:X28"/>
-    <mergeCell ref="Z19:Z28"/>
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="D17:D18"/>
@@ -4349,6 +4347,11 @@
     <mergeCell ref="H6:H15"/>
     <mergeCell ref="J6:J15"/>
     <mergeCell ref="E4:L4"/>
+    <mergeCell ref="S17:Z17"/>
+    <mergeCell ref="AA17:AD17"/>
+    <mergeCell ref="V19:V28"/>
+    <mergeCell ref="X19:X28"/>
+    <mergeCell ref="Z19:Z28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4368,529 +4371,529 @@
   <sheetData>
     <row r="4" spans="5:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="5:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="38" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="40"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="44"/>
     </row>
     <row r="6" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="38" t="s">
+      <c r="G6" s="44"/>
+      <c r="H6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="38" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="40"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="38" t="s">
+      <c r="N6" s="44"/>
+      <c r="O6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="38" t="s">
+      <c r="P6" s="44"/>
+      <c r="Q6" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="40"/>
+      <c r="R6" s="44"/>
       <c r="S6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="U6" s="40"/>
-      <c r="V6" s="38" t="s">
+      <c r="U6" s="44"/>
+      <c r="V6" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="38" t="s">
+      <c r="W6" s="44"/>
+      <c r="X6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="40"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="44"/>
       <c r="AA6" s="21"/>
     </row>
     <row r="7" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="42">
         <v>240</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="46" t="s">
+      <c r="G7" s="44"/>
+      <c r="H7" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="46">
+      <c r="I7" s="46"/>
+      <c r="J7" s="45">
         <v>1E-4</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="46"/>
       <c r="L7" s="20">
         <v>16</v>
       </c>
-      <c r="M7" s="46">
+      <c r="M7" s="45">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="N7" s="47"/>
-      <c r="O7" s="38">
+      <c r="N7" s="46"/>
+      <c r="O7" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="46">
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45">
         <v>200</v>
       </c>
-      <c r="R7" s="47"/>
+      <c r="R7" s="46"/>
       <c r="S7" s="20">
         <v>83</v>
       </c>
-      <c r="T7" s="38">
+      <c r="T7" s="42">
         <v>0.86</v>
       </c>
-      <c r="U7" s="40"/>
-      <c r="V7" s="38">
+      <c r="U7" s="44"/>
+      <c r="V7" s="42">
         <v>16</v>
       </c>
-      <c r="W7" s="40"/>
-      <c r="X7" s="38">
+      <c r="W7" s="44"/>
+      <c r="X7" s="42">
         <v>0.88061</v>
       </c>
-      <c r="Y7" s="39"/>
-      <c r="Z7" s="40"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="44"/>
       <c r="AA7" s="21"/>
     </row>
     <row r="8" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="42">
         <v>240</v>
       </c>
-      <c r="G8" s="40"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
       <c r="L8" s="20">
         <v>16</v>
       </c>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="38" t="s">
+      <c r="M8" s="47"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="49"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="48"/>
       <c r="S8" s="20">
         <v>199</v>
       </c>
-      <c r="T8" s="38">
+      <c r="T8" s="42">
         <v>0.875</v>
       </c>
-      <c r="U8" s="40"/>
-      <c r="V8" s="38">
+      <c r="U8" s="44"/>
+      <c r="V8" s="42">
         <v>150</v>
       </c>
-      <c r="W8" s="40"/>
-      <c r="X8" s="38">
+      <c r="W8" s="44"/>
+      <c r="X8" s="42">
         <v>0.87702999999999998</v>
       </c>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="40"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="44"/>
       <c r="AA8" s="21"/>
     </row>
     <row r="9" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="42">
         <v>240</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="20">
         <v>32</v>
       </c>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="38">
+      <c r="M9" s="47"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="49"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="48"/>
       <c r="S9" s="20">
         <v>103</v>
       </c>
-      <c r="T9" s="38">
+      <c r="T9" s="42">
         <v>0.875</v>
       </c>
-      <c r="U9" s="40"/>
-      <c r="V9" s="38">
+      <c r="U9" s="44"/>
+      <c r="V9" s="42">
         <v>85</v>
       </c>
-      <c r="W9" s="40"/>
-      <c r="X9" s="38">
+      <c r="W9" s="44"/>
+      <c r="X9" s="42">
         <v>0.88134999999999997</v>
       </c>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="40"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="44"/>
       <c r="AA9" s="21"/>
     </row>
     <row r="10" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="42">
         <v>240</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
       <c r="L10" s="20">
         <v>32</v>
       </c>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="38" t="s">
+      <c r="M10" s="47"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="49"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="48"/>
       <c r="S10" s="20">
         <v>150</v>
       </c>
-      <c r="T10" s="38">
+      <c r="T10" s="42">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U10" s="40"/>
-      <c r="V10" s="38">
+      <c r="U10" s="44"/>
+      <c r="V10" s="42">
         <v>78</v>
       </c>
-      <c r="W10" s="40"/>
-      <c r="X10" s="38">
+      <c r="W10" s="44"/>
+      <c r="X10" s="42">
         <v>0.88275000000000003</v>
       </c>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="40"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="44"/>
       <c r="AA10" s="21"/>
     </row>
     <row r="11" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="42">
         <v>240</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="49"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
       <c r="L11" s="20">
         <v>64</v>
       </c>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="38">
+      <c r="M11" s="47"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="49"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="48"/>
       <c r="S11" s="20">
         <v>199</v>
       </c>
-      <c r="T11" s="38">
+      <c r="T11" s="42">
         <v>0.874</v>
       </c>
-      <c r="U11" s="40"/>
-      <c r="V11" s="38">
+      <c r="U11" s="44"/>
+      <c r="V11" s="42">
         <v>147</v>
       </c>
-      <c r="W11" s="40"/>
-      <c r="X11" s="38">
+      <c r="W11" s="44"/>
+      <c r="X11" s="42">
         <v>0.87795000000000001</v>
       </c>
-      <c r="Y11" s="39"/>
-      <c r="Z11" s="40"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="44"/>
       <c r="AA11" s="21"/>
     </row>
     <row r="12" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="42">
         <v>240</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
       <c r="L12" s="20">
         <v>64</v>
       </c>
-      <c r="M12" s="48"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="38" t="s">
+      <c r="M12" s="47"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="49"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="48"/>
       <c r="S12" s="20">
         <v>114</v>
       </c>
-      <c r="T12" s="38">
+      <c r="T12" s="42">
         <v>0.85899999999999999</v>
       </c>
-      <c r="U12" s="40"/>
-      <c r="V12" s="38">
+      <c r="U12" s="44"/>
+      <c r="V12" s="42">
         <v>59</v>
       </c>
-      <c r="W12" s="40"/>
-      <c r="X12" s="38">
+      <c r="W12" s="44"/>
+      <c r="X12" s="42">
         <v>0.87651000000000001</v>
       </c>
-      <c r="Y12" s="39"/>
-      <c r="Z12" s="40"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="44"/>
       <c r="AA12" s="21"/>
     </row>
     <row r="13" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="42">
         <v>256</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="49"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="20">
         <v>16</v>
       </c>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="38">
+      <c r="M13" s="47"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="49"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="48"/>
       <c r="S13" s="20">
         <v>83</v>
       </c>
-      <c r="T13" s="38">
+      <c r="T13" s="42">
         <v>0.86</v>
       </c>
-      <c r="U13" s="40"/>
-      <c r="V13" s="38">
+      <c r="U13" s="44"/>
+      <c r="V13" s="42">
         <v>16</v>
       </c>
-      <c r="W13" s="40"/>
-      <c r="X13" s="38">
+      <c r="W13" s="44"/>
+      <c r="X13" s="42">
         <v>0.88161</v>
       </c>
-      <c r="Y13" s="39"/>
-      <c r="Z13" s="40"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="44"/>
       <c r="AA13" s="21"/>
     </row>
     <row r="14" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="42">
         <v>256</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="48"/>
       <c r="L14" s="20">
         <v>16</v>
       </c>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="38" t="s">
+      <c r="M14" s="47"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="49"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="48"/>
       <c r="S14" s="20">
         <v>199</v>
       </c>
-      <c r="T14" s="38">
+      <c r="T14" s="42">
         <v>0.875</v>
       </c>
-      <c r="U14" s="40"/>
-      <c r="V14" s="38">
+      <c r="U14" s="44"/>
+      <c r="V14" s="42">
         <v>150</v>
       </c>
-      <c r="W14" s="40"/>
-      <c r="X14" s="38">
+      <c r="W14" s="44"/>
+      <c r="X14" s="42">
         <v>0.87702999999999998</v>
       </c>
-      <c r="Y14" s="39"/>
-      <c r="Z14" s="40"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="44"/>
       <c r="AA14" s="21"/>
     </row>
     <row r="15" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E15" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="42">
         <v>256</v>
       </c>
-      <c r="G15" s="40"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="49"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="48"/>
       <c r="L15" s="20">
         <v>32</v>
       </c>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="38">
+      <c r="M15" s="47"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="49"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="48"/>
       <c r="S15" s="20">
         <v>103</v>
       </c>
-      <c r="T15" s="38">
+      <c r="T15" s="42">
         <v>0.875</v>
       </c>
-      <c r="U15" s="40"/>
-      <c r="V15" s="38">
+      <c r="U15" s="44"/>
+      <c r="V15" s="42">
         <v>85</v>
       </c>
-      <c r="W15" s="40"/>
-      <c r="X15" s="38">
+      <c r="W15" s="44"/>
+      <c r="X15" s="42">
         <v>0.88134999999999997</v>
       </c>
-      <c r="Y15" s="39"/>
-      <c r="Z15" s="40"/>
+      <c r="Y15" s="43"/>
+      <c r="Z15" s="44"/>
       <c r="AA15" s="21"/>
     </row>
     <row r="16" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="42">
         <v>256</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="51"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="50"/>
       <c r="L16" s="20">
         <v>32</v>
       </c>
-      <c r="M16" s="50"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="38" t="s">
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="51"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="50"/>
       <c r="S16" s="20">
         <v>130</v>
       </c>
-      <c r="T16" s="38">
+      <c r="T16" s="42">
         <v>0.86799999999999999</v>
       </c>
-      <c r="U16" s="40"/>
-      <c r="V16" s="38">
+      <c r="U16" s="44"/>
+      <c r="V16" s="42">
         <v>78</v>
       </c>
-      <c r="W16" s="40"/>
-      <c r="X16" s="38">
+      <c r="W16" s="44"/>
+      <c r="X16" s="42">
         <v>0.88275000000000003</v>
       </c>
-      <c r="Y16" s="39"/>
-      <c r="Z16" s="40"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="44"/>
       <c r="AA16" s="21"/>
     </row>
     <row r="17" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="38" t="s">
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="44"/>
+      <c r="S17" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="40"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="42"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="43"/>
+      <c r="Y17" s="44"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="52"/>
     </row>
     <row r="18" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="19" t="s">
@@ -4899,47 +4902,47 @@
       <c r="F18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="38" t="s">
+      <c r="H18" s="44"/>
+      <c r="I18" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="38" t="s">
+      <c r="J18" s="44"/>
+      <c r="K18" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="39"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="38" t="s">
+      <c r="L18" s="43"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="38" t="s">
+      <c r="O18" s="44"/>
+      <c r="P18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="40"/>
+      <c r="Q18" s="44"/>
       <c r="R18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="S18" s="38" t="s">
+      <c r="S18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="T18" s="40"/>
-      <c r="U18" s="38" t="s">
+      <c r="T18" s="44"/>
+      <c r="U18" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="V18" s="40"/>
-      <c r="W18" s="38" t="s">
+      <c r="V18" s="44"/>
+      <c r="W18" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="X18" s="40"/>
+      <c r="X18" s="44"/>
       <c r="Y18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="42"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="52"/>
     </row>
     <row r="19" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="22" t="s">
@@ -4948,43 +4951,43 @@
       <c r="F19" s="20">
         <v>240</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="47"/>
-      <c r="I19" s="46">
+      <c r="H19" s="46"/>
+      <c r="I19" s="45">
         <v>1E-4</v>
       </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="38">
+      <c r="J19" s="46"/>
+      <c r="K19" s="42">
         <v>16</v>
       </c>
-      <c r="L19" s="39"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="46">
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="45">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O19" s="47"/>
-      <c r="P19" s="38">
+      <c r="O19" s="46"/>
+      <c r="P19" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="52">
+      <c r="Q19" s="44"/>
+      <c r="R19" s="53">
         <v>200</v>
       </c>
-      <c r="S19" s="38"/>
-      <c r="T19" s="40"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="38">
+      <c r="S19" s="42"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="42">
         <v>24</v>
       </c>
-      <c r="X19" s="40"/>
+      <c r="X19" s="44"/>
       <c r="Y19" s="20">
         <v>0.87990000000000002</v>
       </c>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="42"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="52"/>
     </row>
     <row r="20" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="22" t="s">
@@ -4993,35 +4996,35 @@
       <c r="F20" s="20">
         <v>240</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="38">
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="42">
         <v>16</v>
       </c>
-      <c r="L20" s="39"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="38" t="s">
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="40"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="38">
+      <c r="Q20" s="44"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="42">
         <v>38</v>
       </c>
-      <c r="X20" s="40"/>
+      <c r="X20" s="44"/>
       <c r="Y20" s="20">
         <v>0.88602999999999998</v>
       </c>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="42"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="52"/>
     </row>
     <row r="21" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="22" t="s">
@@ -5030,35 +5033,35 @@
       <c r="F21" s="20">
         <v>240</v>
       </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="38">
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="42">
         <v>32</v>
       </c>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="38">
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="40"/>
-      <c r="W21" s="38">
+      <c r="Q21" s="44"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="42">
         <v>168</v>
       </c>
-      <c r="X21" s="40"/>
+      <c r="X21" s="44"/>
       <c r="Y21" s="20">
         <v>0.88941999999999999</v>
       </c>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="42"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="52"/>
     </row>
     <row r="22" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22" s="22" t="s">
@@ -5067,35 +5070,35 @@
       <c r="F22" s="20">
         <v>240</v>
       </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="38">
+      <c r="G22" s="47"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="42">
         <v>32</v>
       </c>
-      <c r="L22" s="39"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="38" t="s">
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="40"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="40"/>
-      <c r="W22" s="38">
+      <c r="Q22" s="44"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="42">
         <v>29</v>
       </c>
-      <c r="X22" s="40"/>
+      <c r="X22" s="44"/>
       <c r="Y22" s="20">
         <v>0.88482000000000005</v>
       </c>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="42"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="52"/>
     </row>
     <row r="23" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="23" t="s">
@@ -5104,35 +5107,35 @@
       <c r="F23" s="24">
         <v>240</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="43">
+      <c r="G23" s="47"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="56">
         <v>64</v>
       </c>
-      <c r="L23" s="44"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="43">
+      <c r="L23" s="57"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="56">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="45"/>
-      <c r="W23" s="43">
+      <c r="Q23" s="58"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="56">
         <v>65</v>
       </c>
-      <c r="X23" s="45"/>
+      <c r="X23" s="58"/>
       <c r="Y23" s="24">
         <v>0.88971</v>
       </c>
-      <c r="Z23" s="41"/>
-      <c r="AA23" s="42"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="52"/>
     </row>
     <row r="24" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E24" s="22" t="s">
@@ -5141,35 +5144,35 @@
       <c r="F24" s="20">
         <v>256</v>
       </c>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="38">
+      <c r="G24" s="47"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="42">
         <v>64</v>
       </c>
-      <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="38" t="s">
+      <c r="L24" s="43"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="38">
+      <c r="Q24" s="44"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="42">
         <v>178</v>
       </c>
-      <c r="X24" s="40"/>
+      <c r="X24" s="44"/>
       <c r="Y24" s="20">
         <v>0.88748000000000005</v>
       </c>
-      <c r="Z24" s="41"/>
-      <c r="AA24" s="42"/>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="52"/>
     </row>
     <row r="25" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="22" t="s">
@@ -5178,35 +5181,35 @@
       <c r="F25" s="20">
         <v>256</v>
       </c>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="38">
+      <c r="G25" s="47"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="42">
         <v>16</v>
       </c>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="38">
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="40"/>
-      <c r="W25" s="38">
+      <c r="Q25" s="44"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="42">
         <v>24</v>
       </c>
-      <c r="X25" s="40"/>
+      <c r="X25" s="44"/>
       <c r="Y25" s="20">
         <v>0.87990000000000002</v>
       </c>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="42"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="52"/>
     </row>
     <row r="26" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="22" t="s">
@@ -5215,35 +5218,35 @@
       <c r="F26" s="20">
         <v>256</v>
       </c>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="38">
+      <c r="G26" s="47"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="42">
         <v>16</v>
       </c>
-      <c r="L26" s="39"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="38" t="s">
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="48"/>
+      <c r="P26" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="38">
+      <c r="Q26" s="44"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="42">
         <v>38</v>
       </c>
-      <c r="X26" s="40"/>
+      <c r="X26" s="44"/>
       <c r="Y26" s="20">
         <v>0.88602999999999998</v>
       </c>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="42"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="52"/>
     </row>
     <row r="27" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="22" t="s">
@@ -5252,35 +5255,35 @@
       <c r="F27" s="20">
         <v>256</v>
       </c>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="38">
+      <c r="G27" s="47"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="42">
         <v>32</v>
       </c>
-      <c r="L27" s="39"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="38">
+      <c r="L27" s="43"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="48"/>
+      <c r="P27" s="42">
         <v>0.93700000000000006</v>
       </c>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="40"/>
-      <c r="W27" s="38">
+      <c r="Q27" s="44"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="42">
         <v>29</v>
       </c>
-      <c r="X27" s="40"/>
+      <c r="X27" s="44"/>
       <c r="Y27" s="20">
         <v>0.87646000000000002</v>
       </c>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="42"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="52"/>
     </row>
     <row r="28" spans="5:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="22" t="s">
@@ -5289,49 +5292,144 @@
       <c r="F28" s="20">
         <v>256</v>
       </c>
-      <c r="G28" s="50"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="38">
+      <c r="G28" s="49"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="42">
         <v>32</v>
       </c>
-      <c r="L28" s="39"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="38" t="s">
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="40"/>
-      <c r="U28" s="38"/>
-      <c r="V28" s="40"/>
-      <c r="W28" s="38">
+      <c r="Q28" s="44"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="42"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="42">
         <v>70</v>
       </c>
-      <c r="X28" s="40"/>
+      <c r="X28" s="44"/>
       <c r="Y28" s="20">
         <v>0.87980000000000003</v>
       </c>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="42"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="E5:R5"/>
-    <mergeCell ref="S5:AA5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="G19:H28"/>
+    <mergeCell ref="I19:J28"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:O28"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:R28"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="E17:R17"/>
+    <mergeCell ref="S17:Y17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="X12:Z12"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I16"/>
     <mergeCell ref="J7:K16"/>
@@ -5356,112 +5454,17 @@
     <mergeCell ref="T10:U10"/>
     <mergeCell ref="V10:W10"/>
     <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="E17:R17"/>
-    <mergeCell ref="S17:Y17"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="G19:H28"/>
-    <mergeCell ref="I19:J28"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:O28"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:R28"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="E5:R5"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Z6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>